<commit_message>
Mise en forme des tableaux
</commit_message>
<xml_diff>
--- a/ExerciceExcel1/Islam_Shafaatul_Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
+++ b/ExerciceExcel1/Islam_Shafaatul_Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\ExerciceExcel1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\GitHub2022\ExerciceExcel1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36B8521E-742D-41F0-BD04-12B2B34B3D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8BC9E9-0D52-4706-A629-87DF616B606E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{48301F0E-D64D-47FA-808E-63785099F8DC}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{48301F0E-D64D-47FA-808E-63785099F8DC}"/>
+    <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11385" xr2:uid="{3E08638B-5460-4498-B989-1389FC2D0724}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultat attendu" sheetId="1" r:id="rId1"/>
@@ -131,12 +132,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,8 +269,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +356,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFECF2F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,18 +779,11 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -976,6 +1005,69 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -983,7 +1075,24 @@
     <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2596,424 +2705,427 @@
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Q2"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="5" customWidth="1"/>
-    <col min="2" max="7" width="11.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" style="5" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" style="5"/>
-    <col min="16" max="16" width="9.140625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="5"/>
-    <col min="18" max="18" width="1.7109375" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
+    <col min="2" max="7" width="11.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" style="2" customWidth="1"/>
+    <col min="9" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="9.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="2"/>
+    <col min="18" max="18" width="1.7109375" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
     </row>
     <row r="3" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:17" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="2:17" s="7" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="49" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="2:17" s="4" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="35" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <v>1988.5</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>2897.35</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>5223.25</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>7996.36</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <f>SUM(C9:F9)</f>
         <v>18105.46</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>5215</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>8309.0499999999993</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>4287.9799999999996</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>9352.64</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <f>SUM(C10:F10)</f>
         <v>27164.67</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>7832.97</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>11299.87</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>8264.81</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <v>13226.47</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="5">
         <f>SUM(C11:F11)</f>
         <v>40624.120000000003</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>2337.81</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>2137.81</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <v>1237.81</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="14">
         <v>3237.81</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="5">
         <f>SUM(C12:F12)</f>
         <v>8951.24</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="16">
         <v>4336.37</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <v>1790.84</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="16">
         <v>1206.77</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="17">
         <v>1628.13</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="6">
         <f>SUM(C13:F13)</f>
         <v>8962.11</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="19">
         <f>SUM(C9:C13)</f>
         <v>21710.65</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="19">
         <f>SUM(D9:D13)</f>
         <v>26434.920000000002</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="19">
         <f>SUM(E9:E13)</f>
         <v>20220.620000000003</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <f>SUM(F9:F13)</f>
         <v>35441.409999999996</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="7">
         <f>SUM(G9:G13)</f>
         <v>103807.6</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="2:17" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="39" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="22">
         <v>12462.87</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>8256.9699999999993</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>10884.65</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="23">
         <v>18995.599999999999</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="8">
         <f>SUM(C18:F18)</f>
         <v>50600.09</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="22">
         <v>2533.2399999999998</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="22">
         <v>5855.47</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <v>8525.14</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="23">
         <v>11253.21</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <f>SUM(C19:F19)</f>
         <v>28167.059999999998</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="25">
         <v>8755.24</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="25">
         <v>7562.22</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="25">
         <v>5221.5600000000004</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="26">
         <v>3256.47</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="9">
         <f>SUM(C20:F20)</f>
         <v>24795.49</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="28">
         <f>SUM(C18:C20)</f>
         <v>23751.35</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="28">
         <f>SUM(D18:D20)</f>
         <v>21674.66</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="28">
         <f>SUM(E18:E20)</f>
         <v>24631.350000000002</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="29">
         <f>SUM(F18:F20)</f>
         <v>33505.279999999999</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="10">
         <f>SUM(G18:G20)</f>
         <v>103562.64</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="31">
         <f>-C21+C14</f>
         <v>-2040.6999999999971</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="31">
         <f t="shared" ref="D25:G25" si="0">-D21+D14</f>
         <v>4760.260000000002</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="31">
         <f t="shared" si="0"/>
         <v>-4410.7299999999996</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="32">
         <f t="shared" si="0"/>
         <v>1936.1299999999974</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="11">
         <f t="shared" si="0"/>
         <v>244.9600000000064</v>
       </c>
@@ -3025,7 +3137,7 @@
     <mergeCell ref="B4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:G25">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3043,341 +3155,345 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
     <col min="9" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
     </row>
     <row r="3" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
     </row>
     <row r="5" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:17" ht="12" x14ac:dyDescent="0.2">
+      <c r="B8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="66" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="62">
         <v>1988.5</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="62">
         <v>2897.35</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="62">
         <v>5223.25</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="62">
         <v>7996.36</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="64">
         <v>18105.46</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="62">
         <v>5215</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="62">
         <v>8309.0499999999993</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="62">
         <v>4287.9799999999996</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="62">
         <v>9352.64</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="64">
         <v>27164.67</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="62">
         <v>7832.97</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="62">
         <v>11299.87</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="62">
         <v>8264.81</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="62">
         <v>13226.47</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="64">
         <v>40624.120000000003</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="62">
         <v>2337.81</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="62">
         <v>2137.81</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="62">
         <v>1237.81</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="62">
         <v>3237.81</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="64">
         <v>8951.24</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="62">
         <v>4336.37</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="62">
         <v>1790.84</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="62">
         <v>1206.77</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="62">
         <v>1628.13</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="64">
         <v>8962.11</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="64">
         <v>21710.65</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="64">
         <v>26434.920000000002</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="64">
         <v>20220.620000000003</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="64">
         <v>35441.409999999996</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="72">
         <v>103807.6</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="2:7" ht="12" x14ac:dyDescent="0.2">
+      <c r="B17" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="76" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="68">
         <v>12462.87</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="68">
         <v>8256.9699999999993</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="68">
         <v>10884.65</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="68">
         <v>18995.599999999999</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="70">
         <v>50600.09</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="68">
         <v>2533.2399999999998</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="68">
         <v>5855.47</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="68">
         <v>8525.14</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="68">
         <v>11253.21</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="70">
         <v>28167.059999999998</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="68">
         <v>8755.24</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="68">
         <v>7562.22</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="68">
         <v>5221.5600000000004</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="68">
         <v>3256.47</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="70">
         <v>24795.49</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="70">
         <v>23751.35</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="70">
         <v>21674.66</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="70">
         <v>24631.350000000002</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="70">
         <v>33505.279999999999</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="71">
         <v>103562.64</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:7" ht="12" x14ac:dyDescent="0.2">
+      <c r="B24" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="74" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="78">
         <v>-2040.6999999999971</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="78">
         <v>4760.260000000002</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="78">
         <v>-4410.7299999999996</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="78">
         <v>1936.1299999999974</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="79">
         <v>244.96</v>
       </c>
     </row>
@@ -3385,8 +3501,12 @@
     <row r="27" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B4:Q4"/>
+  </mergeCells>
   <conditionalFormatting sqref="C25:G25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3403,84 +3523,85 @@
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="51" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="51" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="100" style="51" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="51" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="51"/>
+    <col min="1" max="1" width="1.7109375" style="48" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="48" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="100" style="48" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="48" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="50" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="60"/>
-      <c r="D5" s="54" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="51" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="60"/>
-      <c r="D6" s="55" t="s">
+      <c r="C6" s="57"/>
+      <c r="D6" s="52" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="60"/>
-      <c r="D7" s="54" t="s">
+      <c r="C7" s="57"/>
+      <c r="D7" s="51" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="60"/>
-      <c r="D8" s="56" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="53" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="52"/>
+      <c r="C9" s="49"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="50" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="60"/>
-      <c r="D11" s="54" t="s">
+      <c r="C11" s="57"/>
+      <c r="D11" s="51" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="60"/>
-      <c r="D12" s="55" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="52" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="60"/>
-      <c r="D13" s="57" t="s">
+      <c r="C13" s="57"/>
+      <c r="D13" s="54" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout des graphique(version finale)
</commit_message>
<xml_diff>
--- a/ExerciceExcel1/Islam_Shafaatul_Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
+++ b/ExerciceExcel1/Islam_Shafaatul_Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
@@ -8,11 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\GitHub2022\ExerciceExcel1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8BC9E9-0D52-4706-A629-87DF616B606E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6171E9F-55C0-44B6-9CF6-42E2A5E2DD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{48301F0E-D64D-47FA-808E-63785099F8DC}"/>
-    <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11385" xr2:uid="{3E08638B-5460-4498-B989-1389FC2D0724}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{07636995-5095-4029-A33D-5904263B02FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultat attendu" sheetId="1" r:id="rId1"/>
@@ -138,7 +136,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,16 +268,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="8"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -293,12 +296,21 @@
     <font>
       <b/>
       <i/>
-      <sz val="8"/>
+      <sz val="9"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,14 +371,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="34">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -773,13 +779,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -990,6 +1087,81 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -998,6 +1170,12 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -1006,68 +1184,38 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="19" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="2" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="20" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="2" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="20" fillId="2" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="20" fillId="2" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="22" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1075,27 +1223,12 @@
     <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
+        <color theme="5" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -2269,6 +2402,3289 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Croissance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> 2009</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$C$24:$F$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Trimestre 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Trimestre 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Trimestre 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Trimestre 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$C$25:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.00\ "$"</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-2040.6999999999971</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4760.260000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4410.7299999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1936.1299999999974</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A184-444B-9568-5EBECBD42521}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1998611184"/>
+        <c:axId val="1998613680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1998611184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1998613680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1998613680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+              <a:headEnd type="none"/>
+              <a:tailEnd w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0\ &quot;$&quot;" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1998611184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent4">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ventes</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> 2009</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="20"/>
+      <c:rotY val="22"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d>
+          <a:contourClr>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d>
+          <a:contourClr>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10506912206006823"/>
+          <c:y val="0.16892627845254243"/>
+          <c:w val="0.78543537920952045"/>
+          <c:h val="0.72399508794140899"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Trimestre 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$9:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Location</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Courantes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assurances</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fournitures</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$C$9:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1988.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5215</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7832.97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2337.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4336.37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99AD-4F69-B0F7-B01001664FF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trimestre 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$9:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Location</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Courantes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assurances</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fournitures</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$D$9:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2897.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8309.0499999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11299.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2137.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1790.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-99AD-4F69-B0F7-B01001664FF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Trimestre 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$9:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Location</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Courantes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assurances</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fournitures</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$E$9:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5223.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4287.9799999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8264.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1237.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1206.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-99AD-4F69-B0F7-B01001664FF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Trimestre 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$9:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Location</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Courantes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assurances</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fournitures</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$F$9:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7996.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9352.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13226.47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3237.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1628.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-99AD-4F69-B0F7-B01001664FF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="165"/>
+        <c:gapDepth val="332"/>
+        <c:shape val="box"/>
+        <c:axId val="871791072"/>
+        <c:axId val="871793568"/>
+        <c:axId val="1038243936"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="871791072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="871793568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="871793568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="871791072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2000"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="1038243936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="871793568"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8625044670719092"/>
+          <c:y val="5.1031567668116E-2"/>
+          <c:w val="0.12572571751006695"/>
+          <c:h val="0.37894993696368301"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Dépenses</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> 2009</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="10"/>
+      <c:rotY val="110"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10689249071138834"/>
+          <c:y val="0.18556594218513695"/>
+          <c:w val="0.73099345536353411"/>
+          <c:h val="0.72338583201393947"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Données brutes'!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trimestre 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$18:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Résidentiel</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Automobile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Vie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12462.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2533.2399999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8755.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="cylinder"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B33-4EF6-A094-48F56F734EFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Données brutes'!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trimestre 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$18:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Résidentiel</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Automobile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Vie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8256.9699999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5855.47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7562.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="cylinder"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9B33-4EF6-A094-48F56F734EFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Données brutes'!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trimestre 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$18:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Résidentiel</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Automobile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Vie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$E$18:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10884.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8525.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5221.5600000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="cylinder"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9B33-4EF6-A094-48F56F734EFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Données brutes'!$F$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trimestre 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d>
+              <a:contourClr>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Données brutes'!$B$18:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Résidentiel</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Automobile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Vie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Données brutes'!$F$18:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>18995.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11253.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3256.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="cylinder"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9B33-4EF6-A094-48F56F734EFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="354"/>
+        <c:gapDepth val="188"/>
+        <c:shape val="box"/>
+        <c:axId val="995333360"/>
+        <c:axId val="995334608"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="995333360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="995334608"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="995334608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="995333360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2000"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2362,6 +5778,119 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3897BD6-89F2-B52A-C3CC-A0C1A58C6A8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D261CAA4-5F1D-4C5B-B58F-69470DE26EB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A573721B-1318-4CBB-8C4E-9422BCEFA93E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2702,13 +6231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q2"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="D43" sqref="D43"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2724,24 +6247,24 @@
   <sheetData>
     <row r="1" spans="2:17" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
     </row>
     <row r="3" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2752,24 +6275,24 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
     </row>
     <row r="5" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
@@ -3137,7 +6660,7 @@
     <mergeCell ref="B4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:G25">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3150,368 +6673,377 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:Q28"/>
+  <dimension ref="B1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
     <col min="9" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+    <row r="1" spans="2:17" ht="3.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
     </row>
-    <row r="3" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:17" ht="3.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
     </row>
     <row r="5" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="2:17" ht="12" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+    <row r="7" spans="2:17" ht="3.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="D8" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="66" t="s">
+      <c r="G8" s="92" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="61" t="s">
+    <row r="9" spans="2:17" ht="12" x14ac:dyDescent="0.2">
+      <c r="B9" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="62">
+      <c r="C9" s="86">
         <v>1988.5</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="86">
         <v>2897.35</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="86">
         <v>5223.25</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="87">
         <v>7996.36</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="88">
         <v>18105.46</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C10" s="86">
         <v>5215</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="86">
         <v>8309.0499999999993</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="86">
         <v>4287.9799999999996</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="87">
         <v>9352.64</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="88">
         <v>27164.67</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="62">
+      <c r="C11" s="86">
         <v>7832.97</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="86">
         <v>11299.87</v>
       </c>
-      <c r="E11" s="62">
+      <c r="E11" s="86">
         <v>8264.81</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="87">
         <v>13226.47</v>
       </c>
-      <c r="G11" s="64">
+      <c r="G11" s="88">
         <v>40624.120000000003</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="62">
+      <c r="C12" s="86">
         <v>2337.81</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="86">
         <v>2137.81</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="86">
         <v>1237.81</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="87">
         <v>3237.81</v>
       </c>
-      <c r="G12" s="64">
+      <c r="G12" s="88">
         <v>8951.24</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="61" t="s">
+    <row r="13" spans="2:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="62">
+      <c r="C13" s="89">
         <v>4336.37</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="89">
         <v>1790.84</v>
       </c>
-      <c r="E13" s="62">
+      <c r="E13" s="89">
         <v>1206.77</v>
       </c>
-      <c r="F13" s="62">
+      <c r="F13" s="90">
         <v>1628.13</v>
       </c>
-      <c r="G13" s="64">
+      <c r="G13" s="91">
         <v>8962.11</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="63" t="s">
+    <row r="14" spans="2:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="88">
         <v>21710.65</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="88">
         <v>26434.920000000002</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="88">
         <v>20220.620000000003</v>
       </c>
-      <c r="F14" s="64">
+      <c r="F14" s="94">
         <v>35441.409999999996</v>
       </c>
-      <c r="G14" s="72">
+      <c r="G14" s="95">
         <v>103807.6</v>
       </c>
+      <c r="H14" s="66"/>
     </row>
-    <row r="15" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:7" ht="12" x14ac:dyDescent="0.2">
-      <c r="B17" s="75" t="s">
+    <row r="15" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="65"/>
+    </row>
+    <row r="16" spans="2:17" ht="3.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+      <c r="B17" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="76" t="s">
+      <c r="E17" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="76" t="s">
+      <c r="F17" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="76" t="s">
+      <c r="G17" s="68" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="67" t="s">
+    <row r="18" spans="2:8" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="68">
+      <c r="C18" s="58">
         <v>12462.87</v>
       </c>
-      <c r="D18" s="68">
+      <c r="D18" s="58">
         <v>8256.9699999999993</v>
       </c>
-      <c r="E18" s="68">
+      <c r="E18" s="58">
         <v>10884.65</v>
       </c>
-      <c r="F18" s="68">
+      <c r="F18" s="75">
         <v>18995.599999999999</v>
       </c>
-      <c r="G18" s="70">
+      <c r="G18" s="60">
         <v>50600.09</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="67" t="s">
+    <row r="19" spans="2:8" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="68">
+      <c r="C19" s="58">
         <v>2533.2399999999998</v>
       </c>
-      <c r="D19" s="68">
+      <c r="D19" s="58">
         <v>5855.47</v>
       </c>
-      <c r="E19" s="68">
+      <c r="E19" s="58">
         <v>8525.14</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="75">
         <v>11253.21</v>
       </c>
-      <c r="G19" s="70">
+      <c r="G19" s="60">
         <v>28167.059999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="67" t="s">
+    <row r="20" spans="2:8" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="68">
+      <c r="C20" s="58">
         <v>8755.24</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="58">
         <v>7562.22</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="73">
         <v>5221.5600000000004</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="76">
         <v>3256.47</v>
       </c>
-      <c r="G20" s="70">
+      <c r="G20" s="60">
         <v>24795.49</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="69" t="s">
+    <row r="21" spans="2:8" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="70">
+      <c r="C21" s="72">
         <v>23751.35</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="72">
         <v>21674.66</v>
       </c>
-      <c r="E21" s="70">
+      <c r="E21" s="60">
         <v>24631.350000000002</v>
       </c>
-      <c r="F21" s="70">
+      <c r="F21" s="77">
         <v>33505.279999999999</v>
       </c>
-      <c r="G21" s="71">
+      <c r="G21" s="78">
         <v>103562.64</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:7" ht="12" x14ac:dyDescent="0.2">
-      <c r="B24" s="73" t="s">
+    <row r="22" spans="2:8" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="65"/>
+    </row>
+    <row r="23" spans="2:8" ht="3.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+      <c r="B24" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="74" t="s">
+      <c r="C24" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="74" t="s">
+      <c r="D24" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="74" t="s">
+      <c r="E24" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="74" t="s">
+      <c r="F24" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="74" t="s">
+      <c r="G24" s="70" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="77" t="s">
+    <row r="25" spans="2:8" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="78">
+      <c r="C25" s="63">
         <v>-2040.6999999999971</v>
       </c>
-      <c r="D25" s="78">
+      <c r="D25" s="63">
         <v>4760.260000000002</v>
       </c>
-      <c r="E25" s="78">
+      <c r="E25" s="63">
         <v>-4410.7299999999996</v>
       </c>
-      <c r="F25" s="78">
+      <c r="F25" s="63">
         <v>1936.1299999999974</v>
       </c>
       <c r="G25" s="79">
         <v>244.96</v>
       </c>
+      <c r="H25" s="66"/>
     </row>
-    <row r="26" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:8" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="65"/>
+    </row>
+    <row r="27" spans="2:8" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:8" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:G25">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3519,11 +7051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3537,15 +7065,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="84" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="50" t="s">
@@ -3553,25 +7081,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="57"/>
+      <c r="C5" s="84"/>
       <c r="D5" s="51" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="57"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="52" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="57"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="51" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="57"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="53" t="s">
         <v>27</v>
       </c>
@@ -3580,7 +7108,7 @@
       <c r="C9" s="49"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="84" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="50" t="s">
@@ -3588,19 +7116,19 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="57"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="51" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="57"/>
+      <c r="C12" s="84"/>
       <c r="D12" s="52" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="57"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="54" t="s">
         <v>23</v>
       </c>

</xml_diff>